<commit_message>
Updated backlog with further stories and removed story about setting up Git
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Emails</t>
   </si>
@@ -31,34 +31,58 @@
     <t>Zip files</t>
   </si>
   <si>
-    <t>Use real zip files rather than ones created on the fly</t>
-  </si>
-  <si>
-    <t>Source Control</t>
-  </si>
-  <si>
     <t>Videos</t>
   </si>
   <si>
-    <t>Put individual links to videos on YouTube</t>
-  </si>
-  <si>
     <t>Layout</t>
   </si>
   <si>
-    <t>Remove extra space on right hand side of pages</t>
-  </si>
-  <si>
     <t>Contact Us</t>
   </si>
   <si>
     <t>Prevent double tap of send button</t>
   </si>
   <si>
-    <t>Set up git</t>
-  </si>
-  <si>
     <t>Give all emails a common subject prefix</t>
+  </si>
+  <si>
+    <t>Links to corresponding videos on YouTube or our site (with embedded YouTube videos) beside songs.</t>
+  </si>
+  <si>
+    <t>Put individual links to videos on YouTube on Video pages</t>
+  </si>
+  <si>
+    <t>Investigate embedding YouTube videos on pages</t>
+  </si>
+  <si>
+    <t>Remove extra space on right hand side of pages (centre content)</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Create SPA using AngularJS</t>
+  </si>
+  <si>
+    <t>Social Links</t>
+  </si>
+  <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>Facebook Like</t>
+  </si>
+  <si>
+    <t>Facebook Comment</t>
+  </si>
+  <si>
+    <t>Facebook Share</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Use real zip files rather than ones created on the fly or make sure these don't fail to download</t>
   </si>
 </sst>
 </file>
@@ -397,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,18 +443,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -438,36 +459,77 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
       <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added story to cleanup commented out code to backlog
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Emails</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>Use real zip files rather than ones created on the fly or make sure these don't fail to download</t>
+  </si>
+  <si>
+    <t>Cleanup</t>
+  </si>
+  <si>
+    <t>Remove code that's commented out</t>
   </si>
 </sst>
 </file>
@@ -421,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,6 +538,14 @@
         <v>21</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Removed story about investigating adding email address to from field
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -14,13 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>Emails</t>
-  </si>
-  <si>
-    <t>Investigate having the from address set to the user's email address</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Album Details Page</t>
   </si>
@@ -427,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,58 +442,58 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -511,39 +505,31 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
       <c r="B15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added story about adding featured content area on homepage
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Album Details Page</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>Remove code that's commented out</t>
+  </si>
+  <si>
+    <t>Homepage</t>
+  </si>
+  <si>
+    <t>Featured songs, videos etc</t>
   </si>
 </sst>
 </file>
@@ -421,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,6 +538,14 @@
         <v>22</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Removed the old way of downloading full albums, using dynamically created zip files and replaced with static zip files on the server
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Album Details Page</t>
   </si>
@@ -22,9 +22,6 @@
     <t>Put in back button to list page</t>
   </si>
   <si>
-    <t>Zip files</t>
-  </si>
-  <si>
     <t>Videos</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
   </si>
   <si>
     <t>Others</t>
-  </si>
-  <si>
-    <t>Use real zip files rather than ones created on the fly or make sure these don't fail to download</t>
   </si>
   <si>
     <t>Cleanup</t>
@@ -427,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +443,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -457,18 +451,18 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -478,34 +472,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
       <c r="B10" t="s">
         <v>15</v>
       </c>
@@ -526,8 +517,11 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -536,14 +530,6 @@
       </c>
       <c r="B15" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added common subject prefix for all emails sent via the contact us section of the site
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -34,9 +34,6 @@
     <t>Prevent double tap of send button</t>
   </si>
   <si>
-    <t>Give all emails a common subject prefix</t>
-  </si>
-  <si>
     <t>Links to corresponding videos on YouTube or our site (with embedded YouTube videos) beside songs.</t>
   </si>
   <si>
@@ -83,6 +80,9 @@
   </si>
   <si>
     <t>Featured songs, videos etc</t>
+  </si>
+  <si>
+    <t>Remove content that is no longer used</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A7" sqref="A7:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +443,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -451,12 +451,12 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -464,7 +464,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -476,22 +476,22 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -512,24 +512,24 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
         <v>21</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes plus added test pages for video
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -40,9 +40,6 @@
     <t>Put individual links to videos on YouTube on Video pages</t>
   </si>
   <si>
-    <t>Investigate embedding YouTube videos on pages</t>
-  </si>
-  <si>
     <t>Remove extra space on right hand side of pages (centre content)</t>
   </si>
   <si>
@@ -73,16 +70,19 @@
     <t>Cleanup</t>
   </si>
   <si>
-    <t>Remove code that's commented out</t>
-  </si>
-  <si>
     <t>Homepage</t>
   </si>
   <si>
-    <t>Featured songs, videos etc</t>
-  </si>
-  <si>
     <t>Remove content that is no longer used</t>
+  </si>
+  <si>
+    <t>Featured content section(s)</t>
+  </si>
+  <si>
+    <t>Remove code that's not used any more</t>
+  </si>
+  <si>
+    <t>Put back videos sections with links to YouTube pages if Killa agrees</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D16"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +456,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -464,7 +464,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -477,59 +477,59 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
         <v>20</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed unused code and content and removed test video pages
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Album Details Page</t>
   </si>
@@ -22,9 +22,6 @@
     <t>Put in back button to list page</t>
   </si>
   <si>
-    <t>Videos</t>
-  </si>
-  <si>
     <t>Layout</t>
   </si>
   <si>
@@ -37,9 +34,6 @@
     <t>Links to corresponding videos on YouTube or our site (with embedded YouTube videos) beside songs.</t>
   </si>
   <si>
-    <t>Put individual links to videos on YouTube on Video pages</t>
-  </si>
-  <si>
     <t>Remove extra space on right hand side of pages (centre content)</t>
   </si>
   <si>
@@ -67,19 +61,10 @@
     <t>Others</t>
   </si>
   <si>
-    <t>Cleanup</t>
-  </si>
-  <si>
     <t>Homepage</t>
   </si>
   <si>
-    <t>Remove content that is no longer used</t>
-  </si>
-  <si>
     <t>Featured content section(s)</t>
-  </si>
-  <si>
-    <t>Remove code that's not used any more</t>
   </si>
   <si>
     <t>Put back videos sections with links to YouTube pages if Killa agrees</t>
@@ -421,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,20 +428,20 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -464,15 +449,15 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -484,52 +469,31 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the way that emails are processed.  Now all the sender information is displayed in the message body
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Album Details Page</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>Put back videos sections with links to YouTube pages if Killa agrees</t>
+  </si>
+  <si>
+    <t>Add media player on page</t>
+  </si>
+  <si>
+    <t>Add links to YouTube pages</t>
   </si>
 </sst>
 </file>
@@ -406,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,62 +443,72 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>